<commit_message>
Added debug prints to PostHomeRoute; updated Acceptance Test spreadsheet
</commit_message>
<xml_diff>
--- a/etc/2191-swen-261-03-d-codelords.xlsx
+++ b/etc/2191-swen-261-03-d-codelords.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="37">
   <si>
     <t xml:space="preserve">Instructions</t>
   </si>
@@ -105,16 +105,28 @@
     <t xml:space="preserve">Given that I'm signed in when I view the Home page then I can start a game by selecting a player listed on the Home page.</t>
   </si>
   <si>
+    <t xml:space="preserve">LAO; 09/10/19</t>
+  </si>
+  <si>
     <t xml:space="preserve">Given that the player I selected isn't yet in a game when I select that player then the system will begin a checkers game and assign me as the starting (Red) player and my opponent as the White player.</t>
   </si>
   <si>
     <t xml:space="preserve">Given that the player I selected is already in a game when I select that player then the system will return me to the Home page with an error message.</t>
   </si>
   <si>
+    <t xml:space="preserve">FAIL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JTL; 09/10/19; code to do this exists, but is not functional</t>
+  </si>
+  <si>
     <t xml:space="preserve">Given that I'm waiting for a game when another player selects a game with me then the system will automatically send me to the Game View as the White player.  NOTE: the `home.ftl` HTML includes a `&lt;meta&gt;` tag that tells the browser to refresh the game every 5 seconds; thus you need to update the `GetHomeRoute` controller to handle the situation when a player is assigned a game.</t>
   </si>
   <si>
     <t xml:space="preserve">Given a valid, initial game board when I drag a piece to a white space then the piece should not be droppable.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JTL; 09/10/19; functionality exists but is not called yet</t>
   </si>
   <si>
     <t xml:space="preserve">Given a valid, initial game board when I drag a piece to an occupied space then the piece should not be droppable.</t>
@@ -133,7 +145,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -178,6 +190,12 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -282,7 +300,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -454,10 +472,10 @@
   </sheetPr>
   <dimension ref="A1:H597"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="0" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="D6" activeCellId="0" sqref="D6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="0" topLeftCell="C7" activePane="topRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
+      <selection pane="topRight" activeCell="D11" activeCellId="0" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -599,78 +617,112 @@
       <c r="E8" s="8"/>
       <c r="G8" s="8"/>
     </row>
-    <row r="9" customFormat="false" ht="42.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="10" t="s">
         <v>24</v>
       </c>
       <c r="B9" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="C9" s="12"/>
-      <c r="D9" s="13"/>
+      <c r="C9" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>26</v>
+      </c>
       <c r="E9" s="12"/>
-      <c r="F9" s="13"/>
+      <c r="F9" s="11"/>
       <c r="G9" s="12"/>
-      <c r="H9" s="13"/>
-    </row>
-    <row r="10" customFormat="false" ht="47.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H9" s="11"/>
+    </row>
+    <row r="10" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="9"/>
       <c r="B10" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C10" s="8"/>
+        <v>27</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>18</v>
+      </c>
       <c r="E10" s="8"/>
       <c r="G10" s="8"/>
     </row>
-    <row r="11" customFormat="false" ht="47.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="9"/>
       <c r="B11" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C11" s="8"/>
+        <v>28</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>30</v>
+      </c>
       <c r="E11" s="8"/>
       <c r="G11" s="8"/>
     </row>
-    <row r="12" customFormat="false" ht="94.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="73.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="9"/>
       <c r="B12" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C12" s="8"/>
+        <v>31</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>18</v>
+      </c>
       <c r="E12" s="8"/>
       <c r="G12" s="8"/>
     </row>
-    <row r="13" customFormat="false" ht="31.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="9"/>
       <c r="B13" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="C13" s="8"/>
+      <c r="D13" s="3" t="s">
+        <v>33</v>
+      </c>
       <c r="E13" s="8"/>
       <c r="G13" s="8"/>
     </row>
-    <row r="14" customFormat="false" ht="31.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="9"/>
       <c r="B14" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C14" s="8"/>
+        <v>34</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D14" s="13" t="s">
+        <v>33</v>
+      </c>
       <c r="E14" s="8"/>
       <c r="G14" s="8"/>
     </row>
-    <row r="15" customFormat="false" ht="63" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="49.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="9"/>
       <c r="B15" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C15" s="8"/>
+        <v>35</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D15" s="13" t="s">
+        <v>33</v>
+      </c>
       <c r="E15" s="8"/>
       <c r="G15" s="8"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="9"/>
       <c r="B16" s="3" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="C16" s="8"/>
       <c r="E16" s="8"/>

</xml_diff>